<commit_message>
Updating the android app bugs
</commit_message>
<xml_diff>
--- a/MMS/Defect Report/DEFECT REPORT - ANDROID V1.4.xlsx
+++ b/MMS/Defect Report/DEFECT REPORT - ANDROID V1.4.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="100">
   <si>
     <t>Defect ID:</t>
   </si>
@@ -444,6 +444,22 @@
 Actual: allows the special characters and more then 20 digits its accepting.
 Expected: It should be restrict the length of the id and allow certain character and digits only . 
 Notes:-please restrict the special characters also</t>
+  </si>
+  <si>
+    <t>dEFECT</t>
+  </si>
+  <si>
+    <t>MonV1.4: Qrcode: Medias are retrieved using media ID's as QR code</t>
+  </si>
+  <si>
+    <t>1. Choose Place media as the category
+2. Capture an image and save
+3. Select Qrcode option to identify media to link
+4. Enter 'media id' number in Qrcode generator
+5. Scan the Qrcode
+Actual: The media retrieved has the 'media id' entered in the Qrcode generator
+Expected: The app must validate the QRcode and display a message informing that the qr code is not linked to any medias
+Note: When a media Id is given as a input in the Qrcode generator and scanned, the app must validate with the QRcodes present in the database and not with the media Id's</t>
   </si>
 </sst>
 </file>
@@ -1855,10 +1871,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:K6"/>
+  <dimension ref="A4:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1952,6 +1968,35 @@
       <c r="G6" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="346.5">
+      <c r="B7" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="3">
+        <v>42100</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>